<commit_message>
Corrected CAT error rates report
Missind “errcord” column, so rates were coming up as NaN
</commit_message>
<xml_diff>
--- a/Tables_Figures/output/table14_SR2_error_rates_response_counts.xlsx
+++ b/Tables_Figures/output/table14_SR2_error_rates_response_counts.xlsx
@@ -83,16 +83,16 @@
     <t>Singular</t>
   </si>
   <si>
-    <t>Inf (1.2, 1.4)</t>
-  </si>
-  <si>
-    <t>NaN (0, 0)</t>
-  </si>
-  <si>
-    <t>Inf (1.2, 1.8)</t>
-  </si>
-  <si>
-    <t>Inf (0.3, 0.3)</t>
+    <t>5.5 (1.2, 1.4)</t>
+  </si>
+  <si>
+    <t>0 (0, 0)</t>
+  </si>
+  <si>
+    <t>6 (1.2, 1.8)</t>
+  </si>
+  <si>
+    <t>0.6 (0.3, 0.3)</t>
   </si>
   <si>
     <t>5.5 (1.5, 1.5)</t>

</xml_diff>